<commit_message>
Missing text related to scalability
</commit_message>
<xml_diff>
--- a/source/assets/files/DevStackAppraisal.xlsx
+++ b/source/assets/files/DevStackAppraisal.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
   <si>
     <t>Asp.net MVC</t>
   </si>
@@ -204,9 +204,6 @@
   </si>
   <si>
     <t>Lots of boilerlate</t>
-  </si>
-  <si>
-    <t>Only a single thread</t>
   </si>
 </sst>
 </file>
@@ -1693,9 +1690,6 @@
       <c r="Y10">
         <v>5</v>
       </c>
-      <c r="Z10" t="s">
-        <v>61</v>
-      </c>
       <c r="AA10">
         <v>8</v>
       </c>

</xml_diff>